<commit_message>
Extra features of tabs, checkbox and multiple document upload was added
</commit_message>
<xml_diff>
--- a/backend/records.xlsx
+++ b/backend/records.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,265 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>center</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>childNumber</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>classOfStudy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>dateOfBirth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>gender</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>rawText</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>yearOfAdmission</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Naripayur</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BET-BJJ/225</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>4 Standard</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>09 Oct 1996</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Bala Devi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>BETHEL AGRICULTUER
-No.1/D2 8t. Thomas Road, Ma|
-Tirunelvell District, Tan{}
-HILD INTRODU
-1 Name : Bala Devi [
-2 Child Number § BET-BLL/225
-3 Sex - Female
-4 Date of Birth : 09.10.1996
-5§ Country of Residence § India
-6 Year of admission : 2004
-7 Class of study 3 IV Standard
-8 Name of Home : FKC Naripaiyur
-9 Famlly details
-Sl.lNo. Name Age Relationshi|
-1 Karuppasamy 53 Father Sick
-2 \Valli 45 Mother Wood cutter
-3 Rajeswaran 25 Elder brother Married
-4 Paramasivan 23 Elder brother Married
-5 Jegatheeswari 22 Elder sister Married
-8 Umayeswari 15 Elder sister At home
-7 Karthick 13 Elder brother Works as an assistant
-in a shop
-Case history:
-The father of the child is a sickly man unable to do any work. The illiterate mother eamns
-what she can which is barely enough to feed them. The family lives in poverty.
-el o
-Date: For Bethel Agricultural Fellowship</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2004</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Naripayur</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BET-BLL/104</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>4 Standard</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>15 Feb 1998</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>T. Selva Ganesh</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>g
-smm—m. R
-BETHEL AGRICULTURAL FELLOWSHIP
-No.1/D2 8t. Thomas Road, Mal
-Tirunelvell District, Tam)
-CHILD INTRODUC
-Name T. Selva Ganesh
-Child Number : BET-BLL/104
-Sex : Male
-Date of Birth : 15.02.1998
-Country of Residence : India
-Year of admission 2 2005
-Class of study % IV Standard
-Name of Home . FKC Naripayur
-MO
-Family details
-1 Thangapandi 43 Father Palmyrah tapper
-2 Annakodi 38 Mother Housewife
-3 Marimuthu 14 Elder Brother Studying IX Standard
-4 Ramkumar 10 Elder Brother Studying VI Standard
-5 Navaneetha Mari Kannan 7 Younger Brother Studying |l Standard
-Case history:
-The child's father is a palmyrah tapper. The juice of the tall palmyrah tree is tapped and sold
-to make country liquor and sugar. The work is seasonal and the income low and inadequate.
-The father does not get adequate work when it is out of season. The family starves most of
-the days.
-The rate of literace in the village is very low. Due to poverty, the villagers do not give importance
-to the education of their children. They send their children to work as labourers for mean wages
-at salt-pan or elsewhere, to help increase the income of the family.
-The child was admitted to the Bethel Centre to save him from poverty, child labour and give him
-a good future.
-Ll Koo
-Date: For Bethel Agricultural Fellowship</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2005</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pudur</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BET-BJJ/141</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>VIl Standard</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>26 Apr 1994</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Narayana Perumal</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>@ BETHEL AGRICULTURAL FELLOWSHIP
-No.1/D2 St. Thomas Road, Maha
-Tirunelvell District, Tamll
-CHILD INTRODUCTIQ
-1 Name : Narayana Perumal
-2 Child Number : BET-BJJ/141
-3 Sex 3 Male
-4 Date of Birth ; 26.04.1994
-5 Country of Residence s India
-6 Year of admission y 2002
-7 Class of study : VIl Standard
-8 Name of Home A FKC K.C. Pudur
-Family details
-Si.No. Name Relationship
-1 Vaikuntam 34 Father Paimyrah Tree climber f
-2 Muthukani 31 Mother Housewife
-3 Suganya 10 Younger Sister Studying V Standard
-4 Poonkodi 7 Younger Sister Studying lil Standard
-5 Sumitha 4 Younger Sister
-_—— s - - -re————.—
-Case history:
-The father is a palmyrah tree tapper. The work provides seasonal and insufficient income.
-The family suffers much due to poverty and disease.
-el Kee
-Date: For Bethel Agricultural Fellowship</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2002</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>